<commit_message>
- document comment updated
</commit_message>
<xml_diff>
--- a/Socket_Protocol.xlsx
+++ b/Socket_Protocol.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mine\sandbox\mukund\esp32-obd2-dongle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A1BC635-0207-4B5A-A882-0C1482EF6F56}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAE6808D-1F16-45D0-A1BD-89F9B7CDAAB1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11625" xr2:uid="{9B72F885-1D85-4CE8-9826-4F06A7D0B3C9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B72F885-1D85-4CE8-9826-4F06A7D0B3C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>1 Byte</t>
   </si>
@@ -41,9 +41,6 @@
     <t>TimeStamp counter</t>
   </si>
   <si>
-    <t>Frame Length</t>
-  </si>
-  <si>
     <t>2 Bytes</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>Body</t>
+  </si>
+  <si>
+    <t>Frame Length / body length</t>
   </si>
 </sst>
 </file>
@@ -130,13 +130,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -456,18 +456,19 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>7</v>
+      <c r="A1" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -476,71 +477,71 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="3"/>
       <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="3"/>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
+      <c r="A5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
         <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>